<commit_message>
pretty much can filter by datamap by needs more tests
</commit_message>
<xml_diff>
--- a/reader/testdata/test_template.xlsx
+++ b/reader/testdata/test_template.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Another Sheet" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="7">
   <si>
     <t xml:space="preserve">Date:</t>
   </si>
@@ -39,6 +40,9 @@
   </si>
   <si>
     <t xml:space="preserve">Integer:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Department</t>
   </si>
 </sst>
 </file>
@@ -142,14 +146,11 @@
   </sheetPr>
   <dimension ref="A2:AF5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AF4" activeCellId="0" sqref="AF4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -295,10 +296,7 @@
       <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1937,4 +1935,33 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="C9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a new test and commented out an old one
</commit_message>
<xml_diff>
--- a/reader/testdata/test_template.xlsx
+++ b/reader/testdata/test_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="10">
   <si>
     <t xml:space="preserve">Date:</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">Greedy Parrots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VUNT</t>
   </si>
 </sst>
 </file>
@@ -156,14 +159,11 @@
   </sheetPr>
   <dimension ref="A2:IG10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="HM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="HM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IG10" activeCellId="0" sqref="IG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -314,10 +314,7 @@
       <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -1963,17 +1960,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,6 +1982,11 @@
       </c>
       <c r="J9" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>